<commit_message>
create new html style database guidance and update Ward 2021 methods
</commit_message>
<xml_diff>
--- a/data/primary_studies/Ward_2021/intermediate/Ward_2021_methods.xlsx
+++ b/data/primary_studies/Ward_2021/intermediate/Ward_2021_methods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Ward_2021/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB70931-A34A-E240-9346-8E4C399E5E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4374DA-2397-4649-AEAC-5F66FB0EC144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
   <si>
     <t>column_name</t>
   </si>
@@ -392,7 +392,10 @@
     <t>organic carbon</t>
   </si>
   <si>
-    <t>Craft regression or EA</t>
+    <t>modeled</t>
+  </si>
+  <si>
+    <t>Craft regression</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1324,7 @@
   <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1571,7 +1574,7 @@
         <v>10</v>
       </c>
       <c r="S3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="T3" t="b">
         <v>1</v>
@@ -1580,7 +1583,7 @@
         <v>121</v>
       </c>
       <c r="V3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="W3" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
hook script development and methods updates
</commit_message>
<xml_diff>
--- a/data/primary_studies/Ward_2021/intermediate/Ward_2021_methods.xlsx
+++ b/data/primary_studies/Ward_2021/intermediate/Ward_2021_methods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Ward_2021/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4374DA-2397-4649-AEAC-5F66FB0EC144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD2988C-9978-A645-80DC-C387B956E257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,19 +383,19 @@
     <t>compaction quantified</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>direct acid treatment</t>
   </si>
   <si>
     <t>organic carbon</t>
   </si>
   <si>
-    <t>modeled</t>
-  </si>
-  <si>
     <t>Craft regression</t>
+  </si>
+  <si>
+    <t>measured</t>
+  </si>
+  <si>
+    <t>not specified</t>
   </si>
 </sst>
 </file>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1562,7 +1562,7 @@
         <v>60</v>
       </c>
       <c r="M3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="N3">
         <v>550</v>
@@ -1580,13 +1580,13 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
+        <v>120</v>
+      </c>
+      <c r="V3" t="s">
+        <v>122</v>
+      </c>
+      <c r="W3" t="s">
         <v>121</v>
-      </c>
-      <c r="V3" t="s">
-        <v>124</v>
-      </c>
-      <c r="W3" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>